<commit_message>
TimeOut property included for IE Edge Mode browser pop up element, Screenshots were added in Launch and Login WorkFlows
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harih\OneDrive\Documents\UiPath\Journal\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testb\Documents\UiPath\FederalBotFactory\Journal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C64DAD8-AEDF-45BB-B9E9-8E440EEC2102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EFC93A-0D34-4FFA-AA59-2890E06ADA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="211">
   <si>
     <t>Name</t>
   </si>
@@ -655,6 +655,9 @@
   </si>
   <si>
     <t>ColName_Currency</t>
+  </si>
+  <si>
+    <t>TimeOut_IEModeEdgeBrowser</t>
   </si>
 </sst>
 </file>
@@ -713,28 +716,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1050,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1370,8 +1366,8 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" t="s">
@@ -1399,34 +1395,34 @@
     </row>
     <row r="44" spans="1:2" ht="15.5" customHeight="1"/>
     <row r="45" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A45" s="9" t="s">
+      <c r="A45" t="s">
         <v>201</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A46" s="9" t="s">
+      <c r="A46" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A47" s="9" t="s">
+      <c r="A47" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A48" s="9" t="s">
+      <c r="A48" t="s">
         <v>107</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1439,144 +1435,144 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A50" s="6" t="s">
+      <c r="A50" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A51" s="6" t="s">
+      <c r="A51" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A52" s="6" t="s">
+      <c r="A52" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="9" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A53" t="s">
         <v>139</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:2" ht="14.5">
+      <c r="A54" t="s">
         <v>141</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="A55" s="6" t="s">
+    <row r="55" spans="1:2" ht="14.5">
+      <c r="A55" t="s">
         <v>143</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:2" ht="14.5">
+      <c r="A56" t="s">
         <v>145</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="A57" s="6" t="s">
+    <row r="57" spans="1:2" ht="14.5">
+      <c r="A57" t="s">
         <v>147</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="6" customFormat="1" ht="14.5">
-      <c r="A58" s="6" t="s">
+    <row r="58" spans="1:2" ht="14.5">
+      <c r="A58" t="s">
         <v>188</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A59" s="6" t="s">
+    <row r="59" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A59" t="s">
         <v>149</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A60" s="6" t="s">
+    <row r="60" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A60" t="s">
         <v>151</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A61" s="6" t="s">
+    <row r="61" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
         <v>198</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="62" spans="1:2" s="6" customFormat="1" ht="14" customHeight="1"/>
+    <row r="62" spans="1:2" ht="14" customHeight="1"/>
     <row r="63" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A63" s="6" t="s">
+      <c r="A63" t="s">
         <v>133</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A65" s="6" t="s">
+      <c r="A65" t="s">
         <v>86</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A66" s="6" t="s">
+      <c r="A66" t="s">
         <v>87</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="6"/>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A67" s="6" t="s">
+      <c r="A67" t="s">
         <v>88</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B68" s="5"/>
+    </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="B69">
-        <v>3000</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
         <v>113</v>
@@ -1584,7 +1580,7 @@
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B70">
         <v>3000</v>
@@ -1595,527 +1591,536 @@
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B71">
-        <v>2</v>
+        <v>3000</v>
       </c>
       <c r="C71" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" t="s">
+        <v>112</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A73" t="s">
         <v>114</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="74" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A74" t="s">
-        <v>116</v>
-      </c>
-      <c r="B74">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="74" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A76" t="s">
         <v>117</v>
       </c>
-      <c r="B75">
+      <c r="B76">
         <v>3</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="77" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A77" t="s">
+    <row r="77" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A78" t="s">
         <v>119</v>
       </c>
-      <c r="B77">
+      <c r="B78">
         <v>2000</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15" customHeight="1">
-      <c r="A78" t="s">
+    <row r="79" spans="1:3" ht="15" customHeight="1">
+      <c r="A79" t="s">
         <v>121</v>
       </c>
-      <c r="B78">
+      <c r="B79">
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A79" t="s">
+    <row r="80" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A80" t="s">
         <v>122</v>
       </c>
-      <c r="B79">
+      <c r="B80">
         <v>1</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="81" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A81" t="s">
-        <v>120</v>
-      </c>
-      <c r="B81">
-        <v>2000</v>
-      </c>
-      <c r="C81" t="s">
-        <v>113</v>
-      </c>
-    </row>
+    <row r="81" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="82" spans="1:3" ht="14.25" customHeight="1">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B82">
-        <v>10</v>
+        <v>2000</v>
+      </c>
+      <c r="C82" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1">
       <c r="A83" t="s">
+        <v>123</v>
+      </c>
+      <c r="B83">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A84" t="s">
         <v>124</v>
       </c>
-      <c r="B83">
+      <c r="B84">
         <v>1</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="85" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A85" s="6" t="s">
+    <row r="85" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="86" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A86" t="s">
         <v>158</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B86" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="87" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A87" s="6" t="s">
+    <row r="87" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="88" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A88" t="s">
         <v>159</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B88" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="88" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A88" s="6" t="s">
+    <row r="89" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A89" t="s">
         <v>161</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B89" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="90" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A90" s="6" t="s">
+    <row r="90" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="91" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A91" t="s">
         <v>163</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B91" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A91" s="6" t="s">
+    <row r="92" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A92" t="s">
         <v>165</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B92" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="92" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A92" s="6" t="s">
+    <row r="93" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A93" t="s">
         <v>167</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B93" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A93" s="6" t="s">
+    <row r="94" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A94" t="s">
         <v>168</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B94" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="95" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A95" s="6" t="s">
+    <row r="95" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="96" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A96" t="s">
         <v>170</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B96">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A96" s="6" t="s">
+    <row r="97" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A97" t="s">
         <v>171</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B97">
         <v>40000</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C97" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="97" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B97" s="7"/>
-    </row>
-    <row r="98" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A98" s="6" t="s">
+    <row r="98" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A99" t="s">
         <v>172</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B99">
         <v>30000</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C99" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="99" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A99" s="6" t="s">
+    <row r="100" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A100" t="s">
         <v>173</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B100">
         <v>30000</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="C100" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="100" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A100" s="6" t="s">
+    <row r="101" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A101" t="s">
         <v>174</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B101">
         <v>60000</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C101" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="101" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B101" s="7"/>
-    </row>
-    <row r="102" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A102" s="6" t="s">
+    <row r="102" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B102" s="5"/>
+    </row>
+    <row r="103" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A103" t="s">
         <v>119</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B103">
         <v>2000</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C103" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A103" s="6" t="s">
+    <row r="104" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A104" t="s">
         <v>121</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B104">
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A104" s="6" t="s">
+    <row r="105" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A105" t="s">
         <v>122</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B105">
         <v>1</v>
       </c>
-      <c r="C104" s="6" t="s">
+      <c r="C105" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="106" spans="1:3" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A106" s="6" t="s">
+    <row r="106" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="107" spans="1:3" ht="15" customHeight="1">
+      <c r="A107" t="s">
         <v>120</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B107">
         <v>2000</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="C107" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="107" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A107" s="6" t="s">
+    <row r="108" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A108" t="s">
         <v>123</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B108">
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:3" s="6" customFormat="1" ht="17.5" customHeight="1">
-      <c r="A108" s="6" t="s">
+    <row r="109" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A109" t="s">
         <v>124</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B109">
         <v>1</v>
       </c>
-      <c r="C108" s="6" t="s">
+      <c r="C109" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="109" spans="1:3" s="6" customFormat="1" ht="17.5" customHeight="1"/>
-    <row r="110" spans="1:3" s="6" customFormat="1" ht="17.5" customHeight="1">
-      <c r="A110" s="6" t="s">
+    <row r="110" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="111" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A111" t="s">
         <v>175</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B111">
         <v>3000</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="C111" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="112" spans="1:3" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A112" s="6" t="s">
+    <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="113" spans="1:3" ht="14" customHeight="1">
+      <c r="A113" t="s">
         <v>176</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B113">
         <v>1</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C113" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="113" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="114" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A114" s="6" t="s">
+    <row r="114" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="115" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A115" t="s">
         <v>177</v>
       </c>
-      <c r="B114" s="6">
+      <c r="B115">
         <v>60000</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="C115" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A115" s="6" t="s">
+    <row r="116" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A116" t="s">
         <v>178</v>
       </c>
-      <c r="B115" s="6">
+      <c r="B116">
         <v>60000</v>
       </c>
-      <c r="C115" s="6" t="s">
+      <c r="C116" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A116" s="6" t="s">
+    <row r="117" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A117" t="s">
         <v>179</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B117">
         <v>60000</v>
       </c>
-      <c r="C116" s="6" t="s">
+      <c r="C117" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="118" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A118" s="6" t="s">
+    <row r="118" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="119" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A119" t="s">
         <v>110</v>
       </c>
-      <c r="B118" s="7">
+      <c r="B119" s="5">
         <v>2000</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C119" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="119" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A119" s="6" t="s">
+    <row r="120" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A120" t="s">
         <v>112</v>
       </c>
-      <c r="B119" s="6">
+      <c r="B120">
         <v>1</v>
       </c>
-      <c r="C119" s="6" t="s">
+      <c r="C120" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A120" s="6" t="s">
+    <row r="121" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A121" t="s">
         <v>114</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="B121" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="121" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A121" s="6" t="s">
+    <row r="122" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A122" t="s">
         <v>156</v>
       </c>
-      <c r="B121" s="7">
+      <c r="B122" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A122" s="6" t="s">
+    <row r="123" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A123" t="s">
         <v>157</v>
       </c>
-      <c r="B122" s="7">
+      <c r="B123" s="5">
         <v>3</v>
       </c>
-      <c r="C122" s="6" t="s">
+      <c r="C123" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="124" spans="1:3" s="6" customFormat="1" ht="14.5">
-      <c r="A124" s="6" t="s">
+    <row r="124" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="125" spans="1:3" ht="14.5">
+      <c r="A125" t="s">
         <v>73</v>
       </c>
-      <c r="B124" s="6" t="s">
+      <c r="B125" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="125" spans="1:3" s="6" customFormat="1" ht="14.5">
-      <c r="A125" s="6" t="s">
+    <row r="126" spans="1:3" ht="14.5">
+      <c r="A126" t="s">
         <v>74</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="B126" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="126" spans="1:3" s="6" customFormat="1" ht="14.5">
-      <c r="A126" s="6" t="s">
+    <row r="127" spans="1:3" ht="14.5">
+      <c r="A127" t="s">
         <v>77</v>
       </c>
-      <c r="B126" s="7" t="s">
+      <c r="B127" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="127" spans="1:3" s="6" customFormat="1" ht="14.5">
-      <c r="A127" s="6" t="s">
+    <row r="128" spans="1:3" ht="14.5">
+      <c r="A128" t="s">
         <v>79</v>
       </c>
-      <c r="B127" s="7" t="s">
+      <c r="B128" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="128" spans="1:3" s="6" customFormat="1" ht="14.5"/>
-    <row r="129" spans="1:3" s="6" customFormat="1" ht="14.5">
-      <c r="A129" s="6" t="s">
+    <row r="129" spans="1:3" ht="14.5"/>
+    <row r="130" spans="1:3" ht="14.5">
+      <c r="A130" t="s">
         <v>80</v>
       </c>
-      <c r="B129" s="7" t="s">
+      <c r="B130" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="130" spans="1:3" s="6" customFormat="1" ht="29">
-      <c r="A130" s="6" t="s">
+    <row r="131" spans="1:3" ht="29">
+      <c r="A131" t="s">
         <v>82</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B131" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="131" spans="1:3" s="6" customFormat="1" ht="14.5">
-      <c r="A131" s="6" t="s">
+    <row r="132" spans="1:3" ht="14.5">
+      <c r="A132" t="s">
         <v>83</v>
       </c>
-      <c r="B131" s="7">
+      <c r="B132" s="5">
         <v>60</v>
       </c>
-      <c r="C131" s="6" t="s">
+      <c r="C132" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="132" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="133" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A133" s="6" t="s">
+    <row r="133" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="134" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A134" t="s">
         <v>180</v>
       </c>
-      <c r="B133" s="6" t="s">
+      <c r="B134" t="s">
         <v>181</v>
       </c>
-      <c r="C133" s="6" t="s">
+      <c r="C134" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="134" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A134" s="6" t="s">
+    <row r="135" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A135" t="s">
         <v>182</v>
       </c>
-      <c r="B134" s="7" t="s">
+      <c r="B135" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A135" s="6" t="s">
+    <row r="136" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A136" t="s">
         <v>183</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B136" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="136" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A136" s="6" t="s">
+    <row r="137" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A137" t="s">
         <v>66</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C137" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="137" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A137" s="6" t="s">
+    <row r="138" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A138" t="s">
         <v>67</v>
       </c>
-      <c r="B137" s="7">
+      <c r="B138" s="5">
         <v>60000</v>
       </c>
-      <c r="C137" s="6" t="s">
+      <c r="C138" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="138" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="139" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A139" s="6" t="s">
+    <row r="139" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="140" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A140" t="s">
         <v>184</v>
       </c>
-      <c r="B139" s="4"/>
-      <c r="C139" s="6" t="s">
+      <c r="C140" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="140" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A140" s="6" t="s">
+    <row r="141" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A141" t="s">
         <v>185</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="B141" s="5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="141" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A141" s="6" t="s">
+    <row r="142" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A142" t="s">
         <v>186</v>
       </c>
-      <c r="B141" s="8" t="s">
+      <c r="B142" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="143" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="144" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="145" ht="14.25" customHeight="1"/>
@@ -2970,6 +2975,7 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>